<commit_message>
feat: add automatic auth
</commit_message>
<xml_diff>
--- a/Расписание.xlsx
+++ b/Расписание.xlsx
@@ -1,38 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaScript\Learning\FE35-onl\Homework\Timetable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A122AAF-2312-4547-9921-28F03E214083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D28FB4A5-91C6-43B1-AA7F-917035C38E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="2388" windowHeight="564" xr2:uid="{0EC63A4D-95EE-4B91-9A30-DAFA64463890}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Data-table" sheetId="1" r:id="rId1"/>
+    <sheet name="Visual" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="86">
   <si>
     <t>Фасад</t>
   </si>
@@ -178,9 +172,6 @@
     <t>Вечер</t>
   </si>
   <si>
-    <t>После заката</t>
-  </si>
-  <si>
     <t>Вторник</t>
   </si>
   <si>
@@ -199,27 +190,9 @@
     <t>Воскресенье</t>
   </si>
   <si>
-    <t>Офсет таймер</t>
-  </si>
-  <si>
-    <t>Сцена</t>
-  </si>
-  <si>
-    <t>Сцена 2</t>
-  </si>
-  <si>
-    <t>Сцена 3</t>
-  </si>
-  <si>
-    <t>Сцена 4</t>
-  </si>
-  <si>
     <t xml:space="preserve">               ХХ:ХХ</t>
   </si>
   <si>
-    <t xml:space="preserve"> Сцена 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">              ХХ:ХХ</t>
   </si>
   <si>
@@ -251,13 +224,73 @@
   </si>
   <si>
     <t>f8562f11-2919-4b8e-9db8-7578751e5f15</t>
+  </si>
+  <si>
+    <t>Основной</t>
+  </si>
+  <si>
+    <t>Белый статика</t>
+  </si>
+  <si>
+    <t>Белый микс</t>
+  </si>
+  <si>
+    <t>Белый пульсации</t>
+  </si>
+  <si>
+    <t>Цветной динамика</t>
+  </si>
+  <si>
+    <t>Экорежим</t>
+  </si>
+  <si>
+    <t>Лиловый</t>
+  </si>
+  <si>
+    <t>Закат/Рассвет</t>
+  </si>
+  <si>
+    <t>Осень</t>
+  </si>
+  <si>
+    <t>Южный молл</t>
+  </si>
+  <si>
+    <t>Ночь</t>
+  </si>
+  <si>
+    <t>Закрытие ТРЦ</t>
+  </si>
+  <si>
+    <t>Фикс. Время</t>
+  </si>
+  <si>
+    <t>Астро</t>
+  </si>
+  <si>
+    <t>Сценарий</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Сценарий 1</t>
+  </si>
+  <si>
+    <t>Сценарий 2</t>
+  </si>
+  <si>
+    <t>Сценарий 3</t>
+  </si>
+  <si>
+    <t>Сценарий 4</t>
+  </si>
+  <si>
+    <t>Дневное выключение</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,6 +315,13 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF1F497D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -291,7 +331,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -387,11 +427,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -438,6 +515,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,13 +551,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>275475</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>227850</xdr:rowOff>
@@ -485,6 +577,7 @@
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:grayscl/>
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -508,13 +601,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>265950</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>227850</xdr:rowOff>
@@ -557,15 +650,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>275475</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>237375</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -606,6 +699,138 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="208800" cy="208800"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5500465B-80ED-4702-95AF-CAC9DE56A049}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3514725" y="647700"/>
+          <a:ext cx="208800" cy="208800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="208800" cy="208800"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BFD8C25-6FF6-4CF0-999A-3BEF66E78CC5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3505200" y="1638300"/>
+          <a:ext cx="208800" cy="208800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="208800" cy="208800"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82F4E40A-0F69-4956-B0EB-E685DEFF1C20}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3514725" y="2143125"/>
+          <a:ext cx="208800" cy="208800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
       <xdr:row>3</xdr:row>
@@ -614,10 +839,10 @@
     <xdr:ext cx="208800" cy="208800"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
+        <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5500465B-80ED-4702-95AF-CAC9DE56A049}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6115BF3-1D22-48D7-A739-42B88233525F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -658,10 +883,10 @@
     <xdr:ext cx="208800" cy="208800"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6">
+        <xdr:cNvPr id="10" name="Picture 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BFD8C25-6FF6-4CF0-999A-3BEF66E78CC5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFC9F188-A621-4422-9583-FEE4CE8A19A3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -696,16 +921,16 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="208800" cy="208800"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7">
+        <xdr:cNvPr id="11" name="Picture 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82F4E40A-0F69-4956-B0EB-E685DEFF1C20}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2595885F-8CCF-403A-AFED-D015FC636F37}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -746,10 +971,10 @@
     <xdr:ext cx="208800" cy="208800"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8">
+        <xdr:cNvPr id="12" name="Picture 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6115BF3-1D22-48D7-A739-42B88233525F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D499B68-CE33-41CB-805D-48F3BD8AC6D0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -790,10 +1015,10 @@
     <xdr:ext cx="208800" cy="208800"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 9">
+        <xdr:cNvPr id="13" name="Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFC9F188-A621-4422-9583-FEE4CE8A19A3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0A60B37-03C4-467A-A9BF-E827F5E8BD1F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -828,16 +1053,16 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="208800" cy="208800"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 10">
+        <xdr:cNvPr id="14" name="Picture 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2595885F-8CCF-403A-AFED-D015FC636F37}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A24B6A8C-6A62-425B-B733-8EB45E45EB3B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -878,10 +1103,10 @@
     <xdr:ext cx="208800" cy="208800"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Picture 11">
+        <xdr:cNvPr id="15" name="Picture 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D499B68-CE33-41CB-805D-48F3BD8AC6D0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DF84A69-4BA6-4554-ABC3-19CB77F2678B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -922,10 +1147,10 @@
     <xdr:ext cx="208800" cy="208800"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 12">
+        <xdr:cNvPr id="16" name="Picture 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0A60B37-03C4-467A-A9BF-E827F5E8BD1F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A70D7D7-AB3B-4655-90C1-3331033D98F3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -960,16 +1185,16 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="208800" cy="208800"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Picture 13">
+        <xdr:cNvPr id="17" name="Picture 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A24B6A8C-6A62-425B-B733-8EB45E45EB3B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{546DF4A1-51EA-4AAD-8827-31AA19D5F6A0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1003,17 +1228,17 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="208800" cy="208800"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Picture 14">
+        <xdr:cNvPr id="18" name="Picture 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DF84A69-4BA6-4554-ABC3-19CB77F2678B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C441298B-A64F-4060-8A72-2852DFBC936B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1034,7 +1259,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3514725" y="647700"/>
+          <a:off x="8410575" y="904875"/>
           <a:ext cx="208800" cy="208800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1054,10 +1279,10 @@
     <xdr:ext cx="208800" cy="208800"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Picture 15">
+        <xdr:cNvPr id="19" name="Picture 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A70D7D7-AB3B-4655-90C1-3331033D98F3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D257E865-7AD0-40B9-AB40-F7FB94F37AE1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1092,16 +1317,16 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="208800" cy="208800"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Picture 16">
+        <xdr:cNvPr id="20" name="Picture 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{546DF4A1-51EA-4AAD-8827-31AA19D5F6A0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5ADE532-A34E-424F-811A-F2F79F4AD522}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1142,10 +1367,10 @@
     <xdr:ext cx="208800" cy="208800"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Picture 17">
+        <xdr:cNvPr id="21" name="Picture 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C441298B-A64F-4060-8A72-2852DFBC936B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32E20B8F-345E-4D0E-AEEA-9CE68AD10B20}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1166,7 +1391,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8410575" y="904875"/>
+          <a:off x="9391650" y="904875"/>
           <a:ext cx="208800" cy="208800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1186,10 +1411,10 @@
     <xdr:ext cx="208800" cy="208800"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="Picture 18">
+        <xdr:cNvPr id="22" name="Picture 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D257E865-7AD0-40B9-AB40-F7FB94F37AE1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD0503CD-F838-4CC2-9564-0BB136F73182}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1224,16 +1449,16 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="208800" cy="208800"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="Picture 19">
+        <xdr:cNvPr id="23" name="Picture 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5ADE532-A34E-424F-811A-F2F79F4AD522}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5465DE9-21B2-4B4B-BE8D-954E9DEDC45D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1266,18 +1491,18 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>55245</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="208800" cy="208800"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="Picture 20">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32E20B8F-345E-4D0E-AEEA-9CE68AD10B20}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B2209F0-EBC0-494D-BDDC-2F5F9E7F2EF6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1298,95 +1523,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9391650" y="904875"/>
-          <a:ext cx="208800" cy="208800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="208800" cy="208800"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="22" name="Picture 21">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD0503CD-F838-4CC2-9564-0BB136F73182}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3505200" y="1638300"/>
-          <a:ext cx="208800" cy="208800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="208800" cy="208800"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="Picture 22">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5465DE9-21B2-4B4B-BE8D-954E9DEDC45D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3514725" y="2143125"/>
+          <a:off x="3712845" y="914400"/>
           <a:ext cx="208800" cy="208800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1696,10 +1833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB1183FA-8BD4-483A-AFB7-FC52944C7378}">
-  <dimension ref="B2:Q33"/>
+  <dimension ref="B2:Q44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1810,7 +1947,7 @@
         <v>35</v>
       </c>
       <c r="F6" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.3">
@@ -1823,7 +1960,7 @@
         <v>36</v>
       </c>
       <c r="F7" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
@@ -1836,7 +1973,7 @@
         <v>37</v>
       </c>
       <c r="F8" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.3">
@@ -1851,7 +1988,7 @@
         <v>38</v>
       </c>
       <c r="F9" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.3">
@@ -1864,7 +2001,7 @@
         <v>39</v>
       </c>
       <c r="F10" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.3">
@@ -1877,7 +2014,7 @@
         <v>40</v>
       </c>
       <c r="F11" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
@@ -1892,7 +2029,7 @@
         <v>41</v>
       </c>
       <c r="F12" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.3">
@@ -1905,7 +2042,7 @@
         <v>42</v>
       </c>
       <c r="F13" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
@@ -2014,12 +2151,81 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:6" x14ac:dyDescent="0.3">
       <c r="E33" t="s">
         <v>43</v>
       </c>
       <c r="F33" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D36" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E36" s="21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D37" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E37" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D38" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E38" s="20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D39" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="E39" s="20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D40" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="4:6" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="D41" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D42" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E42" s="20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D43" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E43" s="20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="E44" s="20" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -2037,24 +2243,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC58A8E2-C1E4-4DF6-8BC5-2EAA47491B9A}">
-  <dimension ref="D2:L15"/>
+  <dimension ref="C2:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="5" width="14.6640625" customWidth="1"/>
-    <col min="6" max="12" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="11" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="17.44140625" customWidth="1"/>
+    <col min="14" max="14" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="4:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D3" s="9"/>
-      <c r="E3" s="10"/>
+    <row r="2" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="3:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C3" s="9"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="11" t="s">
+        <v>46</v>
+      </c>
       <c r="F3" s="11" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>49</v>
@@ -2071,348 +2283,374 @@
       <c r="K3" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="L3" s="11" t="s">
+    </row>
+    <row r="4" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="4" spans="4:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>63</v>
-      </c>
       <c r="G4" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="4:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="15"/>
-      <c r="E5" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="15"/>
+      <c r="D5" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>54</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="4:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D6" s="16"/>
-      <c r="E6" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="3:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="16"/>
+      <c r="D6" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>81</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="4:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>9</v>
+      <c r="D7" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="4:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="18"/>
-      <c r="E8" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="18"/>
+      <c r="D8" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>55</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="4:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D9" s="19"/>
-      <c r="E9" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="3:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="19"/>
+      <c r="D9" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>82</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="4:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+    </row>
+    <row r="11" spans="3:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="24"/>
+      <c r="D11" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+    </row>
+    <row r="12" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="4:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="18"/>
-      <c r="E11" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="4:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D12" s="19"/>
-      <c r="E12" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="L12" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="4:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="4:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="15"/>
-      <c r="E14" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="K14" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="L14" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="4:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D15" s="16"/>
-      <c r="E15" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="K15" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="L15" s="8" t="s">
-        <v>59</v>
+      <c r="D12" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="18"/>
+      <c r="D13" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="3:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="19"/>
+      <c r="D14" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="15"/>
+      <c r="D16" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="3:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="16"/>
+      <c r="D17" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D15"/>
+  <mergeCells count="5">
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="C10:C11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: rename periods, add daytime and styles
</commit_message>
<xml_diff>
--- a/Расписание.xlsx
+++ b/Расписание.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaScript\Learning\FE35-onl\Homework\Timetable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D28FB4A5-91C6-43B1-AA7F-917035C38E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C9371C-88B3-4E32-BF56-7408DDEAE78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2388" windowHeight="564" xr2:uid="{0EC63A4D-95EE-4B91-9A30-DAFA64463890}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{0EC63A4D-95EE-4B91-9A30-DAFA64463890}"/>
   </bookViews>
   <sheets>
     <sheet name="Data-table" sheetId="1" r:id="rId1"/>
@@ -468,7 +468,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -489,6 +489,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -513,15 +531,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1835,7 +1844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB1183FA-8BD4-483A-AFB7-FC52944C7378}">
   <dimension ref="B2:Q44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
@@ -1848,7 +1857,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
       <c r="D2" t="s">
@@ -1895,8 +1904,8 @@
       </c>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B3" s="13"/>
-      <c r="C3" s="12" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="18" t="s">
         <v>12</v>
       </c>
       <c r="D3" t="s">
@@ -1910,8 +1919,8 @@
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B4" s="13"/>
-      <c r="C4" s="12"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="18"/>
       <c r="D4" t="s">
         <v>10</v>
       </c>
@@ -1923,8 +1932,8 @@
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B5" s="13"/>
-      <c r="C5" s="12"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="18"/>
       <c r="D5" t="s">
         <v>11</v>
       </c>
@@ -1936,8 +1945,8 @@
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B6" s="13"/>
-      <c r="C6" s="13" t="s">
+      <c r="B6" s="19"/>
+      <c r="C6" s="19" t="s">
         <v>13</v>
       </c>
       <c r="D6" t="s">
@@ -1951,8 +1960,8 @@
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
       <c r="D7" t="s">
         <v>10</v>
       </c>
@@ -1964,8 +1973,8 @@
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
       <c r="D8" t="s">
         <v>11</v>
       </c>
@@ -1977,8 +1986,8 @@
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B9" s="13"/>
-      <c r="C9" s="13" t="s">
+      <c r="B9" s="19"/>
+      <c r="C9" s="19" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
@@ -1992,8 +2001,8 @@
       </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
       <c r="D10" t="s">
         <v>10</v>
       </c>
@@ -2005,8 +2014,8 @@
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
       <c r="D11" t="s">
         <v>11</v>
       </c>
@@ -2018,8 +2027,8 @@
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="13"/>
-      <c r="C12" s="12" t="s">
+      <c r="B12" s="19"/>
+      <c r="C12" s="18" t="s">
         <v>15</v>
       </c>
       <c r="D12" t="s">
@@ -2033,8 +2042,8 @@
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B13" s="13"/>
-      <c r="C13" s="12"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="18"/>
       <c r="D13" t="s">
         <v>10</v>
       </c>
@@ -2046,8 +2055,8 @@
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B14" s="13"/>
-      <c r="C14" s="12"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="18"/>
       <c r="D14" t="s">
         <v>11</v>
       </c>
@@ -2160,71 +2169,71 @@
       </c>
     </row>
     <row r="36" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D36" s="21" t="s">
+      <c r="D36" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="E36" s="21" t="s">
+      <c r="E36" s="16" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="37" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D37" s="20" t="s">
+      <c r="D37" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E37" s="20" t="s">
+      <c r="E37" s="15" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="38" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D38" s="20" t="s">
+      <c r="D38" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="E38" s="20" t="s">
+      <c r="E38" s="15" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="39" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D39" s="20" t="s">
+      <c r="D39" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="E39" s="20" t="s">
+      <c r="E39" s="15" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="40" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D40" s="20" t="s">
+      <c r="D40" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="E40" s="20" t="s">
+      <c r="E40" s="15" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="41" spans="4:6" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="D41" s="20" t="s">
+      <c r="D41" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="E41" s="20" t="s">
+      <c r="E41" s="15" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="42" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D42" s="20" t="s">
+      <c r="D42" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="E42" s="20" t="s">
+      <c r="E42" s="15" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="43" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D43" s="20" t="s">
+      <c r="D43" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="E43" s="20" t="s">
+      <c r="E43" s="15" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="44" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="E44" s="20" t="s">
+      <c r="E44" s="15" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2243,10 +2252,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC58A8E2-C1E4-4DF6-8BC5-2EAA47491B9A}">
-  <dimension ref="C2:K17"/>
+  <dimension ref="C2:K33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2285,7 +2294,7 @@
       </c>
     </row>
     <row r="4" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="20" t="s">
         <v>76</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -2314,7 +2323,7 @@
       </c>
     </row>
     <row r="5" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="15"/>
+      <c r="C5" s="21"/>
       <c r="D5" s="4" t="s">
         <v>79</v>
       </c>
@@ -2341,7 +2350,7 @@
       </c>
     </row>
     <row r="6" spans="3:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="16"/>
+      <c r="C6" s="22"/>
       <c r="D6" s="5" t="s">
         <v>80</v>
       </c>
@@ -2368,7 +2377,7 @@
       </c>
     </row>
     <row r="7" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="23" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -2397,7 +2406,7 @@
       </c>
     </row>
     <row r="8" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="18"/>
+      <c r="C8" s="24"/>
       <c r="D8" s="4" t="s">
         <v>79</v>
       </c>
@@ -2424,7 +2433,7 @@
       </c>
     </row>
     <row r="9" spans="3:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="19"/>
+      <c r="C9" s="25"/>
       <c r="D9" s="5" t="s">
         <v>80</v>
       </c>
@@ -2451,35 +2460,35 @@
       </c>
     </row>
     <row r="10" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="26" t="s">
         <v>85</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
     </row>
     <row r="11" spans="3:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="24"/>
+      <c r="C11" s="27"/>
       <c r="D11" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
     </row>
     <row r="12" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="23" t="s">
         <v>47</v>
       </c>
       <c r="D12" s="3" t="s">
@@ -2508,7 +2517,7 @@
       </c>
     </row>
     <row r="13" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="18"/>
+      <c r="C13" s="24"/>
       <c r="D13" s="4" t="s">
         <v>79</v>
       </c>
@@ -2535,7 +2544,7 @@
       </c>
     </row>
     <row r="14" spans="3:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="19"/>
+      <c r="C14" s="25"/>
       <c r="D14" s="5" t="s">
         <v>80</v>
       </c>
@@ -2562,7 +2571,7 @@
       </c>
     </row>
     <row r="15" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="20" t="s">
         <v>77</v>
       </c>
       <c r="D15" s="3" t="s">
@@ -2591,7 +2600,7 @@
       </c>
     </row>
     <row r="16" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="15"/>
+      <c r="C16" s="21"/>
       <c r="D16" s="4" t="s">
         <v>79</v>
       </c>
@@ -2618,7 +2627,7 @@
       </c>
     </row>
     <row r="17" spans="3:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="16"/>
+      <c r="C17" s="22"/>
       <c r="D17" s="5" t="s">
         <v>80</v>
       </c>
@@ -2644,8 +2653,108 @@
         <v>84</v>
       </c>
     </row>
+    <row r="19" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C20" s="20">
+        <v>0</v>
+      </c>
+      <c r="D20" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C21" s="21"/>
+      <c r="D21" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="22"/>
+      <c r="D22" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C23" s="23">
+        <v>4</v>
+      </c>
+      <c r="D23" s="12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C24" s="24"/>
+      <c r="D24" s="13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="25"/>
+      <c r="D25" s="14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C26" s="26">
+        <v>8</v>
+      </c>
+      <c r="D26" s="12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C27" s="27"/>
+      <c r="D27" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C28" s="23">
+        <v>11</v>
+      </c>
+      <c r="D28" s="12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C29" s="24"/>
+      <c r="D29" s="13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C30" s="25"/>
+      <c r="D30" s="14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C31" s="20">
+        <v>15</v>
+      </c>
+      <c r="D31" s="12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C32" s="21"/>
+      <c r="D32" s="13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C33" s="22"/>
+      <c r="D33" s="14">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="10">
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="C31:C33"/>
     <mergeCell ref="C4:C6"/>
     <mergeCell ref="C7:C9"/>
     <mergeCell ref="C12:C14"/>

</xml_diff>

<commit_message>
feat: add colorpicker and homepage
</commit_message>
<xml_diff>
--- a/Расписание.xlsx
+++ b/Расписание.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaScript\Learning\FE35-onl\Homework\Timetable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C9371C-88B3-4E32-BF56-7408DDEAE78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCAD4AB4-EE6E-4818-BA35-7FFF77AF0BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{0EC63A4D-95EE-4B91-9A30-DAFA64463890}"/>
+    <workbookView xWindow="7716" yWindow="0" windowWidth="15264" windowHeight="10872" activeTab="1" xr2:uid="{0EC63A4D-95EE-4B91-9A30-DAFA64463890}"/>
   </bookViews>
   <sheets>
     <sheet name="Data-table" sheetId="1" r:id="rId1"/>
@@ -331,7 +331,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -464,11 +464,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -538,6 +553,21 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1834,7 +1864,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2252,10 +2282,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC58A8E2-C1E4-4DF6-8BC5-2EAA47491B9A}">
-  <dimension ref="C2:K33"/>
+  <dimension ref="B2:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2742,24 +2772,150 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C33" s="22"/>
       <c r="D33" s="14">
         <v>18</v>
       </c>
     </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B36" s="32"/>
+      <c r="C36" s="28">
+        <v>5</v>
+      </c>
+      <c r="D36" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B37" s="32"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B38" s="32"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B39" s="32"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B40" s="32"/>
+      <c r="C40" s="28">
+        <v>10</v>
+      </c>
+      <c r="D40" s="29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B41" s="32"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B42" s="32"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B43" s="32"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="29">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B44" s="32"/>
+      <c r="C44" s="30">
+        <v>15</v>
+      </c>
+      <c r="D44" s="29">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B45" s="32"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="29">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B46" s="32"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="29">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B47" s="32"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="29">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B48" s="32"/>
+      <c r="C48" s="28">
+        <v>20</v>
+      </c>
+      <c r="D48" s="29">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B49" s="32"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="29">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B50" s="32"/>
+      <c r="C50" s="28"/>
+      <c r="D50" s="31">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B51" s="32"/>
+      <c r="C51" s="28"/>
+      <c r="D51" s="31">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="16">
+    <mergeCell ref="B36:B43"/>
+    <mergeCell ref="B44:B51"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="C44:C47"/>
+    <mergeCell ref="C48:C51"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="C10:C11"/>
     <mergeCell ref="C20:C22"/>
     <mergeCell ref="C23:C25"/>
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="C28:C30"/>
     <mergeCell ref="C31:C33"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="C10:C11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix:home page requests fixed
</commit_message>
<xml_diff>
--- a/Расписание.xlsx
+++ b/Расписание.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaScript\Learning\FE35-onl\Homework\Timetable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B5B5DD-DEED-4F12-ADF5-EE5381AAD17E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF91C771-3FD1-4F16-8B3A-40AFAD0EFD94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8316" yWindow="0" windowWidth="13344" windowHeight="11508" activeTab="1" xr2:uid="{0EC63A4D-95EE-4B91-9A30-DAFA64463890}"/>
+    <workbookView xWindow="14664" yWindow="456" windowWidth="7344" windowHeight="11508" xr2:uid="{0EC63A4D-95EE-4B91-9A30-DAFA64463890}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data-table" sheetId="1" r:id="rId1"/>
-    <sheet name="Visual" sheetId="2" r:id="rId2"/>
+    <sheet name="Home" sheetId="3" r:id="rId1"/>
+    <sheet name="Data-table" sheetId="1" r:id="rId2"/>
+    <sheet name="Visual" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="69">
   <si>
     <t>Фасад</t>
   </si>
@@ -76,93 +77,9 @@
     <t>после заката</t>
   </si>
   <si>
-    <t>0d8eb784-f423-4173-a15a-ff1d5da8442c</t>
-  </si>
-  <si>
     <t>Имя</t>
   </si>
   <si>
-    <t>Понедельник время до рассвета</t>
-  </si>
-  <si>
-    <t>Понедельник до рассвета оффсет</t>
-  </si>
-  <si>
-    <t>Понедельник время утро</t>
-  </si>
-  <si>
-    <t>Понедельник утро оффсет</t>
-  </si>
-  <si>
-    <t>Понедельник утро выбор сцены</t>
-  </si>
-  <si>
-    <t>Понедельник до рассвета выбор сцены</t>
-  </si>
-  <si>
-    <t>Понедельник время вечер</t>
-  </si>
-  <si>
-    <t>Понедельник вечер оффсет</t>
-  </si>
-  <si>
-    <t>Понедельник вечер сцена</t>
-  </si>
-  <si>
-    <t>Понедельник время ночь</t>
-  </si>
-  <si>
-    <t>Понедельник ночь оффсет</t>
-  </si>
-  <si>
-    <t>Понедельник ночь сцена</t>
-  </si>
-  <si>
-    <t>ad565a5f-d492-4922-ae6e-31232bbcaf25</t>
-  </si>
-  <si>
-    <t>7e218153-45b2-4044-a828-b37c9a7bed54</t>
-  </si>
-  <si>
-    <t>Mon_TBD_NB</t>
-  </si>
-  <si>
-    <t>Mon_BD_O_NB</t>
-  </si>
-  <si>
-    <t>Mon_BD_S_NB</t>
-  </si>
-  <si>
-    <t>Mon_TM_NB</t>
-  </si>
-  <si>
-    <t>Mon_M_O_NB</t>
-  </si>
-  <si>
-    <t>Mon_M_S_NB</t>
-  </si>
-  <si>
-    <t>Mon_TE_NB</t>
-  </si>
-  <si>
-    <t>Mon_E_O_NB</t>
-  </si>
-  <si>
-    <t>Mon_E_S_NB</t>
-  </si>
-  <si>
-    <t>Mon_TN_NB</t>
-  </si>
-  <si>
-    <t>Mon_N_O_NB</t>
-  </si>
-  <si>
-    <t>Mon_N_S_NB</t>
-  </si>
-  <si>
-    <t>_NB</t>
-  </si>
-  <si>
     <t>Северный молл</t>
   </si>
   <si>
@@ -202,30 +119,6 @@
     <t xml:space="preserve">              07:55</t>
   </si>
   <si>
-    <t>4dc3c06f-f207-43ca-bfab-2a6bce65b554</t>
-  </si>
-  <si>
-    <t>11b6008a-0451-4cba-815c-03ed0c83dc1c</t>
-  </si>
-  <si>
-    <t>eaacc54d-8b70-4e74-bc4a-7bad9a5e248e</t>
-  </si>
-  <si>
-    <t>f1663d29-37db-4ce7-92e7-5563f95156ad</t>
-  </si>
-  <si>
-    <t>06c00f14-a068-4be8-a845-7f92057e768f</t>
-  </si>
-  <si>
-    <t>cb84318d-7c28-4ee7-8336-608d161a3705</t>
-  </si>
-  <si>
-    <t>d9b6ad06-ba73-4dc4-9584-e76c84398f22</t>
-  </si>
-  <si>
-    <t>f8562f11-2919-4b8e-9db8-7578751e5f15</t>
-  </si>
-  <si>
     <t>Основной</t>
   </si>
   <si>
@@ -284,6 +177,63 @@
   </si>
   <si>
     <t>Дневное выключение</t>
+  </si>
+  <si>
+    <t>Home_N_Main_Fb</t>
+  </si>
+  <si>
+    <t>Home_N_LihgtBox_Fb</t>
+  </si>
+  <si>
+    <t>Home_N_W_St_Fb</t>
+  </si>
+  <si>
+    <t>Home_N_logotypes_Fb</t>
+  </si>
+  <si>
+    <t>Home_N_W_Puls_Fb</t>
+  </si>
+  <si>
+    <t>Home_N_W_St+Puls_Fb</t>
+  </si>
+  <si>
+    <t>Home_N_sunset_Fb</t>
+  </si>
+  <si>
+    <t>Home_N_autumn_Fb</t>
+  </si>
+  <si>
+    <t>Home_N_ECO_Fb</t>
+  </si>
+  <si>
+    <t>Home_N_Violet_Fb</t>
+  </si>
+  <si>
+    <t>Home_S_main_Fb</t>
+  </si>
+  <si>
+    <t>Home_S_LihgtBox_Fb</t>
+  </si>
+  <si>
+    <t>Home_S_W_St_Fb</t>
+  </si>
+  <si>
+    <t>Home_S_logotypes_Fb</t>
+  </si>
+  <si>
+    <t>Home_S_W_Puls_Fb</t>
+  </si>
+  <si>
+    <t>Home_S_W_St+Puls_Fb</t>
+  </si>
+  <si>
+    <t>Home_S_Color_dynamic_Fb</t>
+  </si>
+  <si>
+    <t>Home_S_ECO_Fb</t>
+  </si>
+  <si>
+    <t>Home_S_Violet_Fb</t>
   </si>
 </sst>
 </file>
@@ -533,12 +483,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -561,6 +505,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1865,11 +1815,118 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6719B4D-CA1B-4376-84A8-3FE1CDF232C9}">
+  <dimension ref="A3:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.109375" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB1183FA-8BD4-483A-AFB7-FC52944C7378}">
-  <dimension ref="B2:Q44"/>
+  <dimension ref="B2:Q25"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1888,7 +1945,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -1934,12 +1991,6 @@
       </c>
       <c r="D3" t="s">
         <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
@@ -1948,12 +1999,6 @@
       <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B5" s="20"/>
@@ -1961,12 +2006,7 @@
       <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>31</v>
-      </c>
+      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" s="20"/>
@@ -1975,12 +2015,6 @@
       </c>
       <c r="D6" t="s">
         <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.3">
@@ -1989,12 +2023,6 @@
       <c r="D7" t="s">
         <v>10</v>
       </c>
-      <c r="E7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="20"/>
@@ -2002,12 +2030,6 @@
       <c r="D8" t="s">
         <v>11</v>
       </c>
-      <c r="E8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B9" s="20"/>
@@ -2016,12 +2038,6 @@
       </c>
       <c r="D9" t="s">
         <v>9</v>
-      </c>
-      <c r="E9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.3">
@@ -2030,12 +2046,6 @@
       <c r="D10" t="s">
         <v>10</v>
       </c>
-      <c r="E10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B11" s="20"/>
@@ -2043,12 +2053,6 @@
       <c r="D11" t="s">
         <v>11</v>
       </c>
-      <c r="E11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B12" s="20"/>
@@ -2057,12 +2061,6 @@
       </c>
       <c r="D12" t="s">
         <v>9</v>
-      </c>
-      <c r="E12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.3">
@@ -2071,12 +2069,6 @@
       <c r="D13" t="s">
         <v>10</v>
       </c>
-      <c r="E13" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B14" s="20"/>
@@ -2084,181 +2076,74 @@
       <c r="D14" t="s">
         <v>11</v>
       </c>
-      <c r="E14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E20" t="s">
-        <v>44</v>
-      </c>
-      <c r="F20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E22" t="s">
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D17" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D18" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D19" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D20" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="F22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E23" t="s">
+      <c r="E20" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D21" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="F23" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E24" t="s">
+      <c r="E21" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="4:5" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="D22" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="F24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E25" t="s">
+      <c r="E22" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D23" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E26" t="s">
+      <c r="E23" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D24" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="F26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E27" t="s">
-        <v>37</v>
-      </c>
-      <c r="F27" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E28" t="s">
-        <v>38</v>
-      </c>
-      <c r="F28" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E29" t="s">
-        <v>39</v>
-      </c>
-      <c r="F29" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E30" t="s">
-        <v>40</v>
-      </c>
-      <c r="F30" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E31" t="s">
-        <v>41</v>
-      </c>
-      <c r="F31" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E32" t="s">
-        <v>42</v>
-      </c>
-      <c r="F32" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="33" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="E33" t="s">
-        <v>43</v>
-      </c>
-      <c r="F33" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="36" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D36" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="E36" s="16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="37" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D37" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="E37" s="15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="38" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D38" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="E38" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="39" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D39" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="E39" s="15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="40" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D40" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="E40" s="15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="41" spans="4:6" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="D41" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="E41" s="15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="42" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D42" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="E42" s="15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="43" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D43" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="E43" s="15" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="44" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="E44" s="15" t="s">
-        <v>72</v>
+      <c r="E24" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E25" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -2274,11 +2159,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC58A8E2-C1E4-4DF6-8BC5-2EAA47491B9A}">
   <dimension ref="B2:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B44" sqref="B44:B51"/>
     </sheetView>
   </sheetViews>
@@ -2296,199 +2181,199 @@
       <c r="C3" s="9"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="22"/>
+      <c r="D5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="3:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="23"/>
+      <c r="D6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="25"/>
+      <c r="D8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="3:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="26"/>
+      <c r="D9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" s="11" t="s">
+      <c r="F9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="H3" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="24"/>
-      <c r="D5" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="3:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="25"/>
-      <c r="D6" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="27"/>
-      <c r="D8" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="3:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="28"/>
-      <c r="D9" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="29" t="s">
-        <v>85</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
@@ -2499,9 +2384,9 @@
       <c r="K10" s="17"/>
     </row>
     <row r="11" spans="3:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="30"/>
+      <c r="C11" s="28"/>
       <c r="D11" s="4" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
@@ -2512,174 +2397,174 @@
       <c r="K11" s="17"/>
     </row>
     <row r="12" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="25"/>
+      <c r="D13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="3:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="26"/>
+      <c r="D14" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="27"/>
-      <c r="D13" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="K13" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="3:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="28"/>
-      <c r="D14" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>83</v>
-      </c>
       <c r="F14" s="8" t="s">
-        <v>83</v>
+        <v>47</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>83</v>
+        <v>47</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>83</v>
+        <v>47</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>83</v>
+        <v>47</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>83</v>
+        <v>47</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>83</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="23" t="s">
-        <v>77</v>
+      <c r="C15" s="21" t="s">
+        <v>41</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="24"/>
+      <c r="C16" s="22"/>
       <c r="D16" s="4" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="3:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="25"/>
+      <c r="C17" s="23"/>
       <c r="D17" s="5" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="20" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C20" s="23">
+      <c r="C20" s="21">
         <v>0</v>
       </c>
       <c r="D20" s="12">
@@ -2687,19 +2572,19 @@
       </c>
     </row>
     <row r="21" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C21" s="24"/>
+      <c r="C21" s="22"/>
       <c r="D21" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="25"/>
+      <c r="C22" s="23"/>
       <c r="D22" s="14">
         <v>3</v>
       </c>
     </row>
     <row r="23" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C23" s="26">
+      <c r="C23" s="24">
         <v>4</v>
       </c>
       <c r="D23" s="12">
@@ -2707,19 +2592,19 @@
       </c>
     </row>
     <row r="24" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C24" s="27"/>
+      <c r="C24" s="25"/>
       <c r="D24" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="25" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C25" s="28"/>
+      <c r="C25" s="26"/>
       <c r="D25" s="14">
         <v>7</v>
       </c>
     </row>
     <row r="26" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C26" s="29">
+      <c r="C26" s="27">
         <v>8</v>
       </c>
       <c r="D26" s="12">
@@ -2727,13 +2612,13 @@
       </c>
     </row>
     <row r="27" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C27" s="30"/>
+      <c r="C27" s="28"/>
       <c r="D27" s="13">
         <v>10</v>
       </c>
     </row>
     <row r="28" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C28" s="26">
+      <c r="C28" s="24">
         <v>11</v>
       </c>
       <c r="D28" s="12">
@@ -2741,19 +2626,19 @@
       </c>
     </row>
     <row r="29" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C29" s="27"/>
+      <c r="C29" s="25"/>
       <c r="D29" s="13">
         <v>13</v>
       </c>
     </row>
     <row r="30" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C30" s="28"/>
+      <c r="C30" s="26"/>
       <c r="D30" s="14">
         <v>14</v>
       </c>
     </row>
     <row r="31" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C31" s="23">
+      <c r="C31" s="21">
         <v>15</v>
       </c>
       <c r="D31" s="12">
@@ -2761,22 +2646,22 @@
       </c>
     </row>
     <row r="32" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C32" s="24"/>
+      <c r="C32" s="22"/>
       <c r="D32" s="13">
         <v>17</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C33" s="25"/>
+      <c r="C33" s="23"/>
       <c r="D33" s="14">
         <v>18</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B36" s="22">
+      <c r="B36" s="29">
         <v>0</v>
       </c>
-      <c r="C36" s="21">
+      <c r="C36" s="30">
         <v>2</v>
       </c>
       <c r="D36" s="18">
@@ -2784,29 +2669,29 @@
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B37" s="22"/>
-      <c r="C37" s="21"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="30"/>
       <c r="D37" s="18">
         <v>7</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B38" s="22"/>
-      <c r="C38" s="21"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="30"/>
       <c r="D38" s="18">
         <v>8</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B39" s="22"/>
-      <c r="C39" s="21"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="30"/>
       <c r="D39" s="18">
         <v>9</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B40" s="22"/>
-      <c r="C40" s="21">
+      <c r="B40" s="29"/>
+      <c r="C40" s="30">
         <v>3</v>
       </c>
       <c r="D40" s="18">
@@ -2814,31 +2699,31 @@
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B41" s="22"/>
-      <c r="C41" s="21"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="30"/>
       <c r="D41" s="18">
         <v>11</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B42" s="22"/>
-      <c r="C42" s="21"/>
+      <c r="B42" s="29"/>
+      <c r="C42" s="30"/>
       <c r="D42" s="18">
         <v>12</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B43" s="22"/>
-      <c r="C43" s="21"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="30"/>
       <c r="D43" s="18">
         <v>13</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B44" s="22">
+      <c r="B44" s="29">
         <v>1</v>
       </c>
-      <c r="C44" s="22">
+      <c r="C44" s="29">
         <v>4</v>
       </c>
       <c r="D44" s="18">
@@ -2846,29 +2731,29 @@
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B45" s="22"/>
-      <c r="C45" s="22"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="29"/>
       <c r="D45" s="18">
         <v>15</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B46" s="22"/>
-      <c r="C46" s="22"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="29"/>
       <c r="D46" s="18">
         <v>16</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B47" s="22"/>
-      <c r="C47" s="22"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="29"/>
       <c r="D47" s="18">
         <v>17</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B48" s="22"/>
-      <c r="C48" s="21">
+      <c r="B48" s="29"/>
+      <c r="C48" s="30">
         <v>5</v>
       </c>
       <c r="D48" s="18">
@@ -2876,44 +2761,44 @@
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B49" s="22"/>
-      <c r="C49" s="21"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="30"/>
       <c r="D49" s="18">
         <v>19</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B50" s="22"/>
-      <c r="C50" s="21"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="30"/>
       <c r="D50" s="18">
         <v>20</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B51" s="22"/>
-      <c r="C51" s="21"/>
+      <c r="B51" s="29"/>
+      <c r="C51" s="30"/>
       <c r="D51" s="18">
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="C10:C11"/>
     <mergeCell ref="B36:B43"/>
     <mergeCell ref="B44:B51"/>
     <mergeCell ref="C36:C39"/>
     <mergeCell ref="C40:C43"/>
     <mergeCell ref="C44:C47"/>
     <mergeCell ref="C48:C51"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="C31:C33"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix:if else in fetchMode fixed
</commit_message>
<xml_diff>
--- a/Расписание.xlsx
+++ b/Расписание.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaScript\Learning\FE35-onl\Homework\Timetable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF91C771-3FD1-4F16-8B3A-40AFAD0EFD94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC4DA64-5FEB-402B-A0D2-CF9E2FCEA08B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14664" yWindow="456" windowWidth="7344" windowHeight="11508" xr2:uid="{0EC63A4D-95EE-4B91-9A30-DAFA64463890}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0EC63A4D-95EE-4B91-9A30-DAFA64463890}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="91">
   <si>
     <t>Фасад</t>
   </si>
@@ -234,6 +234,72 @@
   </si>
   <si>
     <t>Home_S_Violet_Fb</t>
+  </si>
+  <si>
+    <t>home.js:497 undefined</t>
+  </si>
+  <si>
+    <t>home.js:496 Home_S_main_Fb</t>
+  </si>
+  <si>
+    <t>home.js:496 Home_N_W_St_Fb</t>
+  </si>
+  <si>
+    <t>home.js:496 Home_S_W_St_Fb</t>
+  </si>
+  <si>
+    <t>home.js:496 Home_N_W_Puls_Fb</t>
+  </si>
+  <si>
+    <t>home.js:496 Home_S_W_Puls_Fb</t>
+  </si>
+  <si>
+    <t>home.js:496 Home_N_W_St+Puls_Fb</t>
+  </si>
+  <si>
+    <t>home.js:496 Home_S_W_St+Puls_Fb</t>
+  </si>
+  <si>
+    <t>home.js:497 127</t>
+  </si>
+  <si>
+    <t>home.js:496 Home_N_sunset_Fb</t>
+  </si>
+  <si>
+    <t>home.js:496 Home_S_Color_dynamic_Fb</t>
+  </si>
+  <si>
+    <t>home.js:496 Home_N_autumn_Fb</t>
+  </si>
+  <si>
+    <t>home.js:496 Home_S_ECO_Fb</t>
+  </si>
+  <si>
+    <t>home.js:496 Home_N_ECO_Fb</t>
+  </si>
+  <si>
+    <t>home.js:496 Home_S_Violet_Fb</t>
+  </si>
+  <si>
+    <t>home.js:496 Home_N_Violet_Fb</t>
+  </si>
+  <si>
+    <t>home.js:496 Home_S_lightbox_Fb</t>
+  </si>
+  <si>
+    <t>home.js:497 144</t>
+  </si>
+  <si>
+    <t>home.js:496 Home_N_lightbox_Fb</t>
+  </si>
+  <si>
+    <t>home.js:496 Home_S_logotypes_Fb</t>
+  </si>
+  <si>
+    <t>home.js:497 145</t>
+  </si>
+  <si>
+    <t>home.js:496 Home_N_logotypes_Fb</t>
   </si>
 </sst>
 </file>
@@ -273,12 +339,18 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="11">
@@ -433,7 +505,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -483,6 +555,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -507,12 +585,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1816,104 +1889,265 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6719B4D-CA1B-4376-84A8-3FE1CDF232C9}">
-  <dimension ref="A3:C18"/>
+  <dimension ref="A3:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.88671875" customWidth="1"/>
     <col min="2" max="2" width="6.109375" customWidth="1"/>
     <col min="3" max="3" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>50</v>
       </c>
       <c r="C3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G3" s="31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>52</v>
       </c>
       <c r="C4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G5" s="31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G7" s="31" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G9" s="31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G11" s="31" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>60</v>
       </c>
       <c r="C12" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>62</v>
       </c>
       <c r="C13" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G13" s="31" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G15" s="31" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="G16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="G17" s="31" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>68</v>
+      </c>
+      <c r="G18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G19" s="31" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G21" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G23" s="31" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G25" s="31" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G27" s="31" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G28" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G29" s="31" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G31" s="31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G33" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G34" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G35" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G36" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G37" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G38" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G39" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G40" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2203,7 +2437,7 @@
       </c>
     </row>
     <row r="4" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="23" t="s">
         <v>40</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -2232,7 +2466,7 @@
       </c>
     </row>
     <row r="5" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="22"/>
+      <c r="C5" s="24"/>
       <c r="D5" s="4" t="s">
         <v>43</v>
       </c>
@@ -2259,7 +2493,7 @@
       </c>
     </row>
     <row r="6" spans="3:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="23"/>
+      <c r="C6" s="25"/>
       <c r="D6" s="5" t="s">
         <v>44</v>
       </c>
@@ -2286,7 +2520,7 @@
       </c>
     </row>
     <row r="7" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="26" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -2315,7 +2549,7 @@
       </c>
     </row>
     <row r="8" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="25"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="4" t="s">
         <v>43</v>
       </c>
@@ -2342,7 +2576,7 @@
       </c>
     </row>
     <row r="9" spans="3:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="26"/>
+      <c r="C9" s="28"/>
       <c r="D9" s="5" t="s">
         <v>44</v>
       </c>
@@ -2369,7 +2603,7 @@
       </c>
     </row>
     <row r="10" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="29" t="s">
         <v>49</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -2384,7 +2618,7 @@
       <c r="K10" s="17"/>
     </row>
     <row r="11" spans="3:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="28"/>
+      <c r="C11" s="30"/>
       <c r="D11" s="4" t="s">
         <v>43</v>
       </c>
@@ -2397,7 +2631,7 @@
       <c r="K11" s="17"/>
     </row>
     <row r="12" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="26" t="s">
         <v>19</v>
       </c>
       <c r="D12" s="3" t="s">
@@ -2426,7 +2660,7 @@
       </c>
     </row>
     <row r="13" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="25"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="4" t="s">
         <v>43</v>
       </c>
@@ -2453,7 +2687,7 @@
       </c>
     </row>
     <row r="14" spans="3:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="26"/>
+      <c r="C14" s="28"/>
       <c r="D14" s="5" t="s">
         <v>44</v>
       </c>
@@ -2480,7 +2714,7 @@
       </c>
     </row>
     <row r="15" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="23" t="s">
         <v>41</v>
       </c>
       <c r="D15" s="3" t="s">
@@ -2509,7 +2743,7 @@
       </c>
     </row>
     <row r="16" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="22"/>
+      <c r="C16" s="24"/>
       <c r="D16" s="4" t="s">
         <v>43</v>
       </c>
@@ -2536,7 +2770,7 @@
       </c>
     </row>
     <row r="17" spans="3:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="23"/>
+      <c r="C17" s="25"/>
       <c r="D17" s="5" t="s">
         <v>44</v>
       </c>
@@ -2564,7 +2798,7 @@
     </row>
     <row r="19" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="20" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C20" s="21">
+      <c r="C20" s="23">
         <v>0</v>
       </c>
       <c r="D20" s="12">
@@ -2572,19 +2806,19 @@
       </c>
     </row>
     <row r="21" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C21" s="22"/>
+      <c r="C21" s="24"/>
       <c r="D21" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="23"/>
+      <c r="C22" s="25"/>
       <c r="D22" s="14">
         <v>3</v>
       </c>
     </row>
     <row r="23" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C23" s="24">
+      <c r="C23" s="26">
         <v>4</v>
       </c>
       <c r="D23" s="12">
@@ -2592,19 +2826,19 @@
       </c>
     </row>
     <row r="24" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C24" s="25"/>
+      <c r="C24" s="27"/>
       <c r="D24" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="25" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C25" s="26"/>
+      <c r="C25" s="28"/>
       <c r="D25" s="14">
         <v>7</v>
       </c>
     </row>
     <row r="26" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C26" s="27">
+      <c r="C26" s="29">
         <v>8</v>
       </c>
       <c r="D26" s="12">
@@ -2612,13 +2846,13 @@
       </c>
     </row>
     <row r="27" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C27" s="28"/>
+      <c r="C27" s="30"/>
       <c r="D27" s="13">
         <v>10</v>
       </c>
     </row>
     <row r="28" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C28" s="24">
+      <c r="C28" s="26">
         <v>11</v>
       </c>
       <c r="D28" s="12">
@@ -2626,19 +2860,19 @@
       </c>
     </row>
     <row r="29" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C29" s="25"/>
+      <c r="C29" s="27"/>
       <c r="D29" s="13">
         <v>13</v>
       </c>
     </row>
     <row r="30" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C30" s="26"/>
+      <c r="C30" s="28"/>
       <c r="D30" s="14">
         <v>14</v>
       </c>
     </row>
     <row r="31" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C31" s="21">
+      <c r="C31" s="23">
         <v>15</v>
       </c>
       <c r="D31" s="12">
@@ -2646,22 +2880,22 @@
       </c>
     </row>
     <row r="32" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C32" s="22"/>
+      <c r="C32" s="24"/>
       <c r="D32" s="13">
         <v>17</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C33" s="23"/>
+      <c r="C33" s="25"/>
       <c r="D33" s="14">
         <v>18</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B36" s="29">
+      <c r="B36" s="21">
         <v>0</v>
       </c>
-      <c r="C36" s="30">
+      <c r="C36" s="22">
         <v>2</v>
       </c>
       <c r="D36" s="18">
@@ -2669,29 +2903,29 @@
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B37" s="29"/>
-      <c r="C37" s="30"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="22"/>
       <c r="D37" s="18">
         <v>7</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B38" s="29"/>
-      <c r="C38" s="30"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="22"/>
       <c r="D38" s="18">
         <v>8</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B39" s="29"/>
-      <c r="C39" s="30"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="22"/>
       <c r="D39" s="18">
         <v>9</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B40" s="29"/>
-      <c r="C40" s="30">
+      <c r="B40" s="21"/>
+      <c r="C40" s="22">
         <v>3</v>
       </c>
       <c r="D40" s="18">
@@ -2699,31 +2933,31 @@
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B41" s="29"/>
-      <c r="C41" s="30"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="22"/>
       <c r="D41" s="18">
         <v>11</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B42" s="29"/>
-      <c r="C42" s="30"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="22"/>
       <c r="D42" s="18">
         <v>12</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B43" s="29"/>
-      <c r="C43" s="30"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="22"/>
       <c r="D43" s="18">
         <v>13</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B44" s="29">
+      <c r="B44" s="21">
         <v>1</v>
       </c>
-      <c r="C44" s="29">
+      <c r="C44" s="21">
         <v>4</v>
       </c>
       <c r="D44" s="18">
@@ -2731,29 +2965,29 @@
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
+      <c r="B45" s="21"/>
+      <c r="C45" s="21"/>
       <c r="D45" s="18">
         <v>15</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B46" s="29"/>
-      <c r="C46" s="29"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="21"/>
       <c r="D46" s="18">
         <v>16</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B47" s="29"/>
-      <c r="C47" s="29"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="21"/>
       <c r="D47" s="18">
         <v>17</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B48" s="29"/>
-      <c r="C48" s="30">
+      <c r="B48" s="21"/>
+      <c r="C48" s="22">
         <v>5</v>
       </c>
       <c r="D48" s="18">
@@ -2761,44 +2995,44 @@
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B49" s="29"/>
-      <c r="C49" s="30"/>
+      <c r="B49" s="21"/>
+      <c r="C49" s="22"/>
       <c r="D49" s="18">
         <v>19</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B50" s="29"/>
-      <c r="C50" s="30"/>
+      <c r="B50" s="21"/>
+      <c r="C50" s="22"/>
       <c r="D50" s="18">
         <v>20</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B51" s="29"/>
-      <c r="C51" s="30"/>
+      <c r="B51" s="21"/>
+      <c r="C51" s="22"/>
       <c r="D51" s="18">
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="C10:C11"/>
     <mergeCell ref="B36:B43"/>
     <mergeCell ref="B44:B51"/>
     <mergeCell ref="C36:C39"/>
     <mergeCell ref="C40:C43"/>
     <mergeCell ref="C44:C47"/>
     <mergeCell ref="C48:C51"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="C31:C33"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>